<commit_message>
Added development branch and updated files
</commit_message>
<xml_diff>
--- a/hyper_param_tuning/architectures_and_hypertuning.xlsx
+++ b/hyper_param_tuning/architectures_and_hypertuning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesm/stock_lstm/hyper_param_tuning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703B0926-0884-384F-9C3D-740A73035253}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939CBEE6-51EE-CF49-A4B7-45FA204A8A1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19260" xr2:uid="{1AC054C2-41B9-094A-9D21-6F265B3DB880}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="47">
   <si>
     <t xml:space="preserve"> True</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>LSTM with grid search</t>
+  </si>
+  <si>
+    <t>CNN Univariate multi sequence</t>
+  </si>
+  <si>
+    <t>cnn: [5.673] 3.6, 4.4, 5.2, 3.0, 3.6, 6.8, 9.9</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -823,6 +829,12 @@
       </c>
       <c r="H12">
         <v>8.0863137638619804</v>
+      </c>
+      <c r="K12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:13">

</xml_diff>